<commit_message>
Implement strictNullable option. Default false. on true, depend " | undefined | null" to type of nullable properties.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoPiniaTask.xlsx
+++ b/meta/program/BlancoPiniaTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoPinia/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704CFAE-F488-2240-BDE0-537B093A1C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D88E6C-C4D2-4D40-8347-8A31E69059F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6980" yWindow="600" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -370,6 +370,26 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>strictNullable</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Nullable な property に対して、? の付与をやめて | undefined | null の定義を行う。false の場合は ? が付与されて | undefined のみ付与される。</t>
+    <rPh sb="7" eb="9">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シュツリョク</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -844,24 +864,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -878,9 +893,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,19 +903,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -919,7 +931,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -934,29 +946,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -965,10 +975,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,8 +990,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
@@ -996,17 +1006,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1378,10 +1385,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1402,7 +1409,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="29" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1427,58 +1434,56 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
+      <c r="F6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="75"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="65"/>
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10"/>
@@ -1490,333 +1495,355 @@
       <c r="G10"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
-      <c r="A14" s="44">
+      <c r="A14" s="36">
         <v>1</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="76" t="s">
+      <c r="E14" s="40"/>
+      <c r="F14" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="78"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
-      <c r="A15" s="49">
+      <c r="A15" s="41">
         <f>A14+1</f>
         <v>2</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="60" t="s">
+      <c r="D15" s="44"/>
+      <c r="E15" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="86" t="s">
+      <c r="F15" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="69"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
-      <c r="A16" s="49">
-        <f t="shared" ref="A16:A24" si="0">A15+1</f>
+      <c r="A16" s="41">
+        <f t="shared" ref="A16:A25" si="0">A15+1</f>
         <v>3</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53" t="s">
+      <c r="D16" s="44"/>
+      <c r="E16" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="69"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49">
+      <c r="A17" s="41">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="55" t="s">
+      <c r="D17" s="44"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49">
+      <c r="A18" s="41">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="54">
+      <c r="D18" s="44"/>
+      <c r="E18" s="46">
         <v>4</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="49">
+      <c r="A19" s="41">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="56" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="49">
+      <c r="A20" s="41">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="58" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:10" ht="66" customHeight="1">
-      <c r="A21" s="49">
+      <c r="A21" s="41">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="61" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="83" t="s">
+      <c r="F21" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="85"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="74"/>
     </row>
     <row r="22" spans="1:10" ht="52" customHeight="1">
-      <c r="A22" s="49">
+      <c r="A22" s="41">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="61" t="s">
+      <c r="D22" s="19"/>
+      <c r="E22" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="74"/>
-    </row>
-    <row r="23" spans="1:10" s="66" customFormat="1" ht="41" customHeight="1">
-      <c r="A23" s="49">
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="64"/>
+    </row>
+    <row r="23" spans="1:10" s="56" customFormat="1" ht="41" customHeight="1">
+      <c r="A23" s="41">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="72" t="s">
+      <c r="D23" s="55"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="74"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="64"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="49">
+      <c r="A24" s="41">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="61" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="62" t="s">
+      <c r="F24" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
+      <c r="A25" s="41">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="33"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1839,14 +1866,14 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F44" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F45" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D24:D28 D14:D22" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D22 D24:D29" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C24:C28 C14:C22" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C22 C24:C29" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>
@@ -1879,10 +1906,10 @@
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1890,63 +1917,63 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B4"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B5"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="B6"/>
-      <c r="C6" s="18"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="32" t="s">
         <v>19</v>
       </c>
       <c r="B7"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="32" t="s">
         <v>20</v>
       </c>
       <c r="B8"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="32" t="s">
         <v>21</v>
       </c>
       <c r="B9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="40"/>
+      <c r="A10" s="32"/>
       <c r="B10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="40"/>
+      <c r="A11" s="32"/>
       <c r="B11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="41"/>
+      <c r="A12" s="33"/>
       <c r="B12"/>
     </row>
     <row r="13" spans="1:6">

</xml_diff>